<commit_message>
EPBDS-6472 Allow to mix java and openl classes
--HG--
branch : 5.19.x
</commit_message>
<xml_diff>
--- a/Util/openl-simple-project-archetype/resources/archetype-resources/src/main/openl/rules/TemplateRules.xlsx
+++ b/Util/openl-simple-project-archetype/resources/archetype-resources/src/main/openl/rules/TemplateRules.xlsx
@@ -192,7 +192,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="62">
   <si>
     <t>Replace the table below with your own rules</t>
   </si>
@@ -279,6 +279,105 @@
   </si>
   <si>
     <t>Good Night</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>Datatype Person</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>birthDay</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>_DEFAULT_</t>
+  </si>
+  <si>
+    <t>import</t>
+  </si>
+  <si>
+    <t>com.example.beans</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>datatypePackage</t>
+  </si>
+  <si>
+    <t>com.example.beans.openl</t>
+  </si>
+  <si>
+    <t>scope</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Properties</t>
+  </si>
+  <si>
+    <t>Datatype Auto</t>
+  </si>
+  <si>
+    <t>power</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>person</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>case1</t>
+  </si>
+  <si>
+    <t>case2</t>
+  </si>
+  <si>
+    <t>case3</t>
+  </si>
+  <si>
+    <t>= p</t>
+  </si>
+  <si>
+    <t>= au</t>
+  </si>
+  <si>
+    <t>= ad</t>
+  </si>
+  <si>
+    <t>RETURN</t>
+  </si>
+  <si>
+    <t>Calc</t>
+  </si>
+  <si>
+    <t>= $Calc$case1.age + $Calc$case2.power</t>
+  </si>
+  <si>
+    <t>Spreadsheet Integer calculate(Person p, Auto au, Address ad)</t>
   </si>
 </sst>
 </file>
@@ -364,7 +463,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -494,17 +593,86 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color indexed="8"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -518,7 +686,9 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -531,7 +701,9 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -544,14 +716,16 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -563,9 +737,31 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -573,66 +769,6 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -641,8 +777,45 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -652,39 +825,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -986,18 +1144,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J12"/>
+  <dimension ref="B1:J41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.28515625" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
@@ -1006,235 +1164,420 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
     </row>
     <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
     </row>
     <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="9"/>
-      <c r="C6" s="10" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="12" t="s">
+      <c r="F6" s="1"/>
+      <c r="G6" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="12"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="13" t="s">
+      <c r="H6" s="37"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="27" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="14"/>
-      <c r="C7" s="15" t="s">
+      <c r="B7" s="8"/>
+      <c r="C7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="13" t="s">
+      <c r="F7" s="1"/>
+      <c r="G7" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="13" t="s">
+      <c r="I7" s="1"/>
+      <c r="J7" s="29" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="13" t="s">
+      <c r="F8" s="1"/>
+      <c r="G8" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="H8" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="13" t="s">
+      <c r="I8" s="1"/>
+      <c r="J8" s="29" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="22">
+      <c r="C9" s="16">
         <v>0</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="17">
         <v>11</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="13">
+      <c r="F9" s="1"/>
+      <c r="G9" s="30">
         <v>7</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H9" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="I9" s="4"/>
-      <c r="J9" s="13">
+      <c r="I9" s="1"/>
+      <c r="J9" s="28">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="20">
         <v>12</v>
       </c>
-      <c r="D10" s="27">
+      <c r="D10" s="21">
         <v>17</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="13">
+      <c r="F10" s="1"/>
+      <c r="G10" s="30">
         <v>13</v>
       </c>
-      <c r="H10" s="13" t="s">
+      <c r="H10" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="13">
+      <c r="I10" s="1"/>
+      <c r="J10" s="28">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="26">
+      <c r="C11" s="20">
         <v>18</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D11" s="21">
         <v>21</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="13">
+      <c r="F11" s="1"/>
+      <c r="G11" s="30">
         <v>21</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="H11" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="I11" s="4"/>
-      <c r="J11" s="13">
+      <c r="I11" s="1"/>
+      <c r="J11" s="28">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="30">
+      <c r="C12" s="24">
         <v>22</v>
       </c>
-      <c r="D12" s="31">
+      <c r="D12" s="25">
         <v>23</v>
       </c>
-      <c r="E12" s="32" t="s">
+      <c r="E12" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="13">
+      <c r="F12" s="1"/>
+      <c r="G12" s="30">
         <v>22</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="H12" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="4"/>
-      <c r="J12" s="13">
+      <c r="I12" s="1"/>
+      <c r="J12" s="28">
         <v>22</v>
       </c>
     </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="40"/>
+      <c r="E17" s="41"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="40"/>
+      <c r="E18" s="41"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="40"/>
+      <c r="E19" s="41"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="40"/>
+      <c r="E20" s="41"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="28">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="28"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" s="28">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" s="28"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="28"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" s="37"/>
+      <c r="D35" s="37"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="42"/>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" s="37"/>
+      <c r="D39" s="37"/>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C40" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="D40" s="42"/>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="D41" s="42"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="16">
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="C36:D36"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="G6:H6"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
EPBDS-6616 Support arrays in a generated interface
--HG--
branch : 5.19.x
</commit_message>
<xml_diff>
--- a/Util/openl-simple-project-archetype/resources/archetype-resources/src/main/openl/rules/TemplateRules.xlsx
+++ b/Util/openl-simple-project-archetype/resources/archetype-resources/src/main/openl/rules/TemplateRules.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="For testing" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -192,192 +193,204 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="66">
   <si>
     <t>Replace the table below with your own rules</t>
   </si>
   <si>
+    <t>Rule</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>RET1</t>
+  </si>
+  <si>
+    <t>min &lt;= hour</t>
+  </si>
+  <si>
+    <t>hour &lt;= max</t>
+  </si>
+  <si>
+    <t>greeting</t>
+  </si>
+  <si>
+    <t>Test hello helloTest</t>
+  </si>
+  <si>
+    <t>Run hello helloRun</t>
+  </si>
+  <si>
+    <t>int min</t>
+  </si>
+  <si>
+    <t>int max</t>
+  </si>
+  <si>
+    <t>String greeting</t>
+  </si>
+  <si>
+    <t>hour</t>
+  </si>
+  <si>
+    <t>_res_</t>
+  </si>
+  <si>
+    <t>From</t>
+  </si>
+  <si>
+    <t>To</t>
+  </si>
+  <si>
+    <t>Greeting</t>
+  </si>
+  <si>
+    <t>Hour</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>Good Morning</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>Good Afternoon</t>
+  </si>
+  <si>
+    <t>R30</t>
+  </si>
+  <si>
+    <t>Good Evening</t>
+  </si>
+  <si>
+    <t>R40</t>
+  </si>
+  <si>
+    <t>Good Night</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>Datatype Person</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>birthDay</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>_DEFAULT_</t>
+  </si>
+  <si>
+    <t>import</t>
+  </si>
+  <si>
+    <t>com.example.beans</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>datatypePackage</t>
+  </si>
+  <si>
+    <t>com.example.beans.openl</t>
+  </si>
+  <si>
+    <t>scope</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Properties</t>
+  </si>
+  <si>
+    <t>Datatype Auto</t>
+  </si>
+  <si>
+    <t>power</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>person</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>case1</t>
+  </si>
+  <si>
+    <t>case2</t>
+  </si>
+  <si>
+    <t>case3</t>
+  </si>
+  <si>
+    <t>= p</t>
+  </si>
+  <si>
+    <t>= au</t>
+  </si>
+  <si>
+    <t>= ad</t>
+  </si>
+  <si>
+    <t>RETURN</t>
+  </si>
+  <si>
+    <t>Calc</t>
+  </si>
+  <si>
+    <t>= $Calc$case1.age + $Calc$case2.power</t>
+  </si>
+  <si>
+    <t>Spreadsheet Integer calculate(Person p, Auto au, Address ad)</t>
+  </si>
+  <si>
+    <t>Spreadsheet Integer calculate(Person[] p, Auto[][] au, Address[][][] ad, int[] ar1, Double[][] ar2)</t>
+  </si>
+  <si>
+    <t>Spreadsheet Long[] calculate(Person[] p, Auto[][] au, Address[][][] ad, int[] ar1)</t>
+  </si>
+  <si>
+    <t>= null</t>
+  </si>
+  <si>
+    <t>Spreadsheet DoubleValue[][] calculate(IntValue[] p, ByteValue au, BigDecimal[][][] ad)</t>
+  </si>
+  <si>
     <t>Rules String hello(int hour)</t>
-  </si>
-  <si>
-    <t>Rule</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>RET1</t>
-  </si>
-  <si>
-    <t>min &lt;= hour</t>
-  </si>
-  <si>
-    <t>hour &lt;= max</t>
-  </si>
-  <si>
-    <t>greeting</t>
-  </si>
-  <si>
-    <t>Test hello helloTest</t>
-  </si>
-  <si>
-    <t>Run hello helloRun</t>
-  </si>
-  <si>
-    <t>int min</t>
-  </si>
-  <si>
-    <t>int max</t>
-  </si>
-  <si>
-    <t>String greeting</t>
-  </si>
-  <si>
-    <t>hour</t>
-  </si>
-  <si>
-    <t>_res_</t>
-  </si>
-  <si>
-    <t>From</t>
-  </si>
-  <si>
-    <t>To</t>
-  </si>
-  <si>
-    <t>Greeting</t>
-  </si>
-  <si>
-    <t>Hour</t>
-  </si>
-  <si>
-    <t>Result</t>
-  </si>
-  <si>
-    <t>R10</t>
-  </si>
-  <si>
-    <t>Good Morning</t>
-  </si>
-  <si>
-    <t>R20</t>
-  </si>
-  <si>
-    <t>Good Afternoon</t>
-  </si>
-  <si>
-    <t>R30</t>
-  </si>
-  <si>
-    <t>Good Evening</t>
-  </si>
-  <si>
-    <t>R40</t>
-  </si>
-  <si>
-    <t>Good Night</t>
-  </si>
-  <si>
-    <t>Integer</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>Datatype Person</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>birthDay</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>address</t>
-  </si>
-  <si>
-    <t>_DEFAULT_</t>
-  </si>
-  <si>
-    <t>import</t>
-  </si>
-  <si>
-    <t>com.example.beans</t>
-  </si>
-  <si>
-    <t>Environment</t>
-  </si>
-  <si>
-    <t>datatypePackage</t>
-  </si>
-  <si>
-    <t>com.example.beans.openl</t>
-  </si>
-  <si>
-    <t>scope</t>
-  </si>
-  <si>
-    <t>Module</t>
-  </si>
-  <si>
-    <t>Properties</t>
-  </si>
-  <si>
-    <t>Datatype Auto</t>
-  </si>
-  <si>
-    <t>power</t>
-  </si>
-  <si>
-    <t>String</t>
-  </si>
-  <si>
-    <t>model</t>
-  </si>
-  <si>
-    <t>Person</t>
-  </si>
-  <si>
-    <t>person</t>
-  </si>
-  <si>
-    <t>Step</t>
-  </si>
-  <si>
-    <t>case1</t>
-  </si>
-  <si>
-    <t>case2</t>
-  </si>
-  <si>
-    <t>case3</t>
-  </si>
-  <si>
-    <t>= p</t>
-  </si>
-  <si>
-    <t>= au</t>
-  </si>
-  <si>
-    <t>= ad</t>
-  </si>
-  <si>
-    <t>RETURN</t>
-  </si>
-  <si>
-    <t>Calc</t>
-  </si>
-  <si>
-    <t>= $Calc$case1.age + $Calc$case2.power</t>
-  </si>
-  <si>
-    <t>Spreadsheet Integer calculate(Person p, Auto au, Address ad)</t>
   </si>
 </sst>
 </file>
@@ -777,7 +790,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -842,6 +855,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1147,7 +1163,7 @@
   <dimension ref="B1:J41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1189,7 +1205,7 @@
     </row>
     <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="37" t="s">
-        <v>1</v>
+        <v>65</v>
       </c>
       <c r="C4" s="37"/>
       <c r="D4" s="37"/>
@@ -1202,16 +1218,16 @@
     </row>
     <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -1221,75 +1237,75 @@
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="C6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="E6" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H6" s="37"/>
       <c r="I6" s="1"/>
       <c r="J6" s="27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="8"/>
       <c r="C7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="E7" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>13</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="29" t="s">
         <v>14</v>
-      </c>
-      <c r="H7" s="29" t="s">
-        <v>15</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="E8" s="14" t="s">
         <v>17</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>18</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="29" t="s">
         <v>19</v>
-      </c>
-      <c r="H8" s="29" t="s">
-        <v>20</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="16">
         <v>0</v>
@@ -1298,14 +1314,14 @@
         <v>11</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="30">
         <v>7</v>
       </c>
       <c r="H9" s="31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="28">
@@ -1314,7 +1330,7 @@
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="20">
         <v>12</v>
@@ -1323,14 +1339,14 @@
         <v>17</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="30">
         <v>13</v>
       </c>
       <c r="H10" s="31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="28">
@@ -1339,7 +1355,7 @@
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="20">
         <v>18</v>
@@ -1348,14 +1364,14 @@
         <v>21</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="30">
         <v>21</v>
       </c>
       <c r="H11" s="31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="28">
@@ -1364,7 +1380,7 @@
     </row>
     <row r="12" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="24">
         <v>22</v>
@@ -1373,14 +1389,14 @@
         <v>23</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="30">
         <v>22</v>
       </c>
       <c r="H12" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="28">
@@ -1389,7 +1405,7 @@
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C15" s="37"/>
       <c r="D15" s="37"/>
@@ -1397,67 +1413,67 @@
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D16" s="38"/>
       <c r="E16" s="38"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C17" s="39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D17" s="40"/>
       <c r="E17" s="41"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C18" s="39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D18" s="40"/>
       <c r="E18" s="41"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C19" s="39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D19" s="40"/>
       <c r="E19" s="41"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" s="39" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D20" s="40"/>
       <c r="E20" s="41"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" s="37"/>
       <c r="D23" s="37"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="28" t="s">
         <v>29</v>
-      </c>
-      <c r="C24" s="28" t="s">
-        <v>30</v>
       </c>
       <c r="D24" s="28">
         <v>18</v>
@@ -1465,37 +1481,37 @@
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="28" t="s">
         <v>32</v>
-      </c>
-      <c r="C25" s="28" t="s">
-        <v>33</v>
       </c>
       <c r="D25" s="28"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="28" t="s">
+      <c r="D26" s="28" t="s">
         <v>35</v>
-      </c>
-      <c r="D26" s="28" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C29" s="37"/>
       <c r="D29" s="37"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D30" s="28">
         <v>150</v>
@@ -1503,60 +1519,60 @@
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="28" t="s">
         <v>47</v>
-      </c>
-      <c r="C31" s="28" t="s">
-        <v>48</v>
       </c>
       <c r="D31" s="28"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="28" t="s">
         <v>49</v>
-      </c>
-      <c r="C32" s="28" t="s">
-        <v>50</v>
       </c>
       <c r="D32" s="28"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C35" s="37"/>
       <c r="D35" s="37"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" s="42" t="s">
         <v>37</v>
-      </c>
-      <c r="C36" s="42" t="s">
-        <v>38</v>
       </c>
       <c r="D36" s="42"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C39" s="37"/>
       <c r="D39" s="37"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40" s="42" t="s">
         <v>40</v>
-      </c>
-      <c r="C40" s="42" t="s">
-        <v>41</v>
       </c>
       <c r="D40" s="42"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C41" s="42" t="s">
         <v>42</v>
-      </c>
-      <c r="C41" s="42" t="s">
-        <v>43</v>
       </c>
       <c r="D41" s="42"/>
     </row>
@@ -1582,4 +1598,220 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:E27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9:E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="40"/>
+      <c r="E6" s="41"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="40"/>
+      <c r="E7" s="41"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="40"/>
+      <c r="E8" s="41"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="39">
+        <f>43</f>
+        <v>43</v>
+      </c>
+      <c r="D9" s="40"/>
+      <c r="E9" s="41"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="40"/>
+      <c r="E15" s="41"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="40"/>
+      <c r="E16" s="41"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="40"/>
+      <c r="E17" s="41"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="40"/>
+      <c r="E18" s="41"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="40"/>
+      <c r="E24" s="41"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="40"/>
+      <c r="E25" s="41"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="40"/>
+      <c r="E26" s="41"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="40"/>
+      <c r="E27" s="41"/>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>